<commit_message>
Code updated 23-01-30 11:03:11
</commit_message>
<xml_diff>
--- a/0_历史总表/中国心历史结算总表_81.xlsx
+++ b/0_历史总表/中国心历史结算总表_81.xlsx
@@ -38777,7 +38777,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>"心灵有为 1"</t>
+          <t>心灵有为</t>
         </is>
       </c>
       <c r="C509" t="inlineStr">
@@ -47015,7 +47015,7 @@
       </c>
       <c r="B636" t="inlineStr">
         <is>
-          <t>AdyYouTubeSs</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="C636" t="inlineStr">
@@ -48301,7 +48301,7 @@
       </c>
       <c r="B659" t="inlineStr">
         <is>
-          <t>Rename</t>
+          <t>Disparaître</t>
         </is>
       </c>
       <c r="C659" t="inlineStr">
@@ -48409,7 +48409,7 @@
       </c>
       <c r="B661" t="inlineStr">
         <is>
-          <t>Player-58340439</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="C661" t="inlineStr">

</xml_diff>